<commit_message>
Update SDD_ver1+phan chia.docx Update Weekly_Report_Son.xlsx
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Son.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Son.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="620" windowWidth="21160" windowHeight="17420"/>
+    <workbookView xWindow="405" yWindow="615" windowWidth="19440" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
@@ -409,13 +409,13 @@
     <t>Chưa hoàn thành</t>
   </si>
   <si>
-    <t>Viết SDD cho 4 chức năng Multilanguage và Profile</t>
+    <t xml:space="preserve">     </t>
   </si>
   <si>
-    <t>Viết SDD cho 4 chức năng Login/Logout và Register</t>
+    <t>Viết SDD cho 2 chức năng Login/Logout và Register</t>
   </si>
   <si>
-    <t xml:space="preserve">     </t>
+    <t>Viết SDD cho 2 chức năng Multilanguage và Profile</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3142,27 +3142,27 @@
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="32.625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.375" style="3" customWidth="1"/>
     <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="5.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="6.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="5.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="6.125" style="3" customWidth="1"/>
     <col min="11" max="11" width="6" style="3" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="3" customWidth="1"/>
-    <col min="17" max="1024" width="10.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="5.875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="5.625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="24.375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="3" customWidth="1"/>
+    <col min="17" max="1024" width="10.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
@@ -3228,7 +3228,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1024">
+    <row r="3" spans="1:1024" ht="15">
       <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" s="11" customFormat="1" ht="39">
+    <row r="4" spans="1:1024" s="11" customFormat="1" ht="42.75">
       <c r="A4" s="16">
         <v>41173</v>
       </c>
@@ -4304,7 +4304,7 @@
       <c r="AMI4" s="10"/>
       <c r="AMJ4" s="10"/>
     </row>
-    <row r="5" spans="1:1024" s="11" customFormat="1" ht="26">
+    <row r="5" spans="1:1024" s="11" customFormat="1" ht="28.5">
       <c r="A5" s="16">
         <v>41173</v>
       </c>
@@ -7418,7 +7418,7 @@
       <c r="AMI7" s="10"/>
       <c r="AMJ7" s="10"/>
     </row>
-    <row r="8" spans="1:1024" s="11" customFormat="1">
+    <row r="8" spans="1:1024" s="11" customFormat="1" ht="28.5">
       <c r="A8" s="16">
         <v>41180</v>
       </c>
@@ -8456,7 +8456,7 @@
       <c r="AMI8" s="10"/>
       <c r="AMJ8" s="10"/>
     </row>
-    <row r="9" spans="1:1024" s="11" customFormat="1" ht="26">
+    <row r="9" spans="1:1024" s="11" customFormat="1" ht="28.5">
       <c r="A9" s="16">
         <v>41185</v>
       </c>
@@ -9492,12 +9492,12 @@
       <c r="AMI9" s="10"/>
       <c r="AMJ9" s="10"/>
     </row>
-    <row r="10" spans="1:1024" s="11" customFormat="1" ht="26">
+    <row r="10" spans="1:1024" s="11" customFormat="1" ht="28.5">
       <c r="A10" s="16">
         <v>41186</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>44</v>
@@ -10534,7 +10534,7 @@
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -24918,24 +24918,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="6.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="4.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="6.125" style="3" customWidth="1"/>
     <col min="11" max="11" width="6" style="3" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="3" customWidth="1"/>
-    <col min="17" max="1024" width="10.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="5.875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="5.625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="24.375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="3" customWidth="1"/>
+    <col min="17" max="1024" width="10.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -24999,7 +24999,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" ht="15">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Update báo cáo và i18n cho trang admin
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Son.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Son.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="675" windowWidth="19440" windowHeight="11700"/>
+    <workbookView xWindow="405" yWindow="735" windowWidth="19440" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <definedName name="Excel_BuiltIn__FilterDatabase">Task!$A$4:$F$11</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Task!$A$1:$N$32</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>Project</t>
   </si>
@@ -427,7 +427,37 @@
     <t>Hiện thực login + register</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>28/11/12</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa login + register</t>
+  </si>
+  <si>
+    <t>Việt hóa cho website (dịch các thuật ngữ sang tiếng Việt)</t>
+  </si>
+  <si>
+    <t>Trang chủ + register + login có hỗ trợ tiếng Việt</t>
+  </si>
+  <si>
+    <t>Việt hóa thông báo lỗi</t>
+  </si>
+  <si>
+    <t>Thông báo lỗi trang login và register có hỗ trợ tiếng Việt</t>
+  </si>
+  <si>
+    <t>Bổ sung đa ngôn ngữ cho trang admin</t>
+  </si>
+  <si>
+    <t>Bổ sung trường cho user + thêm đa ngôn ngữ</t>
+  </si>
+  <si>
+    <t>Bổ sung báo cáo</t>
+  </si>
+  <si>
+    <t>Giới thiệu về Ruby + RoR</t>
+  </si>
+  <si>
+    <t>Hoàn chỉnh báo cáo</t>
   </si>
 </sst>
 </file>
@@ -3154,7 +3184,7 @@
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -12617,14 +12647,22 @@
       <c r="AMJ12" s="10"/>
     </row>
     <row r="13" spans="1:1024" s="11" customFormat="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="16" t="s">
         <v>52</v>
       </c>
+      <c r="B13" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="8">
+        <v>5</v>
+      </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -13644,13 +13682,23 @@
       <c r="AMI13" s="10"/>
       <c r="AMJ13" s="10"/>
     </row>
-    <row r="14" spans="1:1024" s="11" customFormat="1">
-      <c r="A14" s="16"/>
-      <c r="B14" s="8"/>
+    <row r="14" spans="1:1024" s="11" customFormat="1" ht="28.5">
+      <c r="A14" s="16">
+        <v>40920</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="8">
+        <v>5</v>
+      </c>
+      <c r="F14" s="8">
+        <v>5</v>
+      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -14670,13 +14718,25 @@
       <c r="AMI14" s="10"/>
       <c r="AMJ14" s="10"/>
     </row>
-    <row r="15" spans="1:1024" s="11" customFormat="1">
-      <c r="A15" s="16"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+    <row r="15" spans="1:1024" s="11" customFormat="1" ht="28.5">
+      <c r="A15" s="16">
+        <v>40951</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="F15" s="8">
+        <v>5</v>
+      </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -15696,13 +15756,25 @@
       <c r="AMI15" s="10"/>
       <c r="AMJ15" s="10"/>
     </row>
-    <row r="16" spans="1:1024" s="11" customFormat="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+    <row r="16" spans="1:1024" s="11" customFormat="1" ht="42.75">
+      <c r="A16" s="16">
+        <v>40980</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="8">
+        <v>3</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -16722,13 +16794,25 @@
       <c r="AMI16" s="10"/>
       <c r="AMJ16" s="10"/>
     </row>
-    <row r="17" spans="1:1024" s="11" customFormat="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+    <row r="17" spans="1:1024" s="11" customFormat="1" ht="28.5">
+      <c r="A17" s="16">
+        <v>40980</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="8">
+        <v>3</v>
+      </c>
+      <c r="F17" s="8">
+        <v>3</v>
+      </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -17749,12 +17833,22 @@
       <c r="AMJ17" s="10"/>
     </row>
     <row r="18" spans="1:1024" s="11" customFormat="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="16">
+        <v>40980</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2</v>
+      </c>
+      <c r="F18" s="8">
+        <v>2</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -18775,12 +18869,22 @@
       <c r="AMJ18" s="10"/>
     </row>
     <row r="19" spans="1:1024" s="11" customFormat="1">
-      <c r="A19" s="16"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="16">
+        <v>41011</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -19801,11 +19905,19 @@
       <c r="AMJ19" s="10"/>
     </row>
     <row r="20" spans="1:1024" s="11" customFormat="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="16">
+        <v>41041</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="E20" s="8">
+        <v>3</v>
+      </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>

</xml_diff>